<commit_message>
Finishing trends tab, still outstanding bugs in data explorer.
</commit_message>
<xml_diff>
--- a/agquery/Update/Policy_Link.xlsx
+++ b/agquery/Update/Policy_Link.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\netid.washington.edu\wfs\EvansEPAR\Project\EPAR\Working Files\RA Working Folders\Claire G\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD24F40-242D-4870-B797-A6B9AC2AE8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69C7243-8192-45DF-9CB3-20F09F626FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="32850" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy_Pathways" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="122">
   <si>
     <t>Goal.Id</t>
   </si>
@@ -289,9 +289,6 @@
     <t>Pathway.Id</t>
   </si>
   <si>
-    <t>Growing vegetables</t>
-  </si>
-  <si>
     <t>feed_cattle</t>
   </si>
   <si>
@@ -422,7 +419,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,14 +555,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF1D1C1D"/>
       <name val="Aptos Narrow"/>
@@ -573,7 +562,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -751,12 +740,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -920,22 +903,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1821,12 +1798,12 @@
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1836,21 +1813,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51:XFD51"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="132.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="132.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1867,1010 +1843,993 @@
         <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30">
+        <v>7</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="3">
-        <v>2</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="4">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="3">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" s="3">
-        <v>3</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D15" s="3">
-        <v>3</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="3">
-        <v>5</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="3">
-        <v>5</v>
-      </c>
-      <c r="E17" s="3" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="3">
-        <v>5</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="3">
-        <v>5</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="3">
-        <v>5</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="3">
-        <v>5</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="3">
-        <v>5</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="3">
-        <v>5</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="3">
-        <v>2</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="3">
-        <v>7</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="3">
-        <v>2</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="3">
-        <v>7</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="3">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="3">
-        <v>7</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="3">
-        <v>2</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="3">
-        <v>7</v>
-      </c>
-      <c r="E27" s="3" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54">
+        <v>9</v>
+      </c>
+      <c r="E54" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="3">
-        <v>2</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="3">
-        <v>7</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="3">
-        <v>2</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="3">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="3">
-        <v>2</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="3">
-        <v>7</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B31" s="3">
-        <v>2</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="3">
-        <v>7</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B32" s="3">
-        <v>2</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="3">
-        <v>7</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="3">
-        <v>2</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="3">
-        <v>7</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="3">
-        <v>2</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="3">
-        <v>7</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="3">
-        <v>2</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="3">
-        <v>8</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="3">
-        <v>2</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="3">
-        <v>8</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="3">
-        <v>2</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="3">
-        <v>8</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B38" s="3">
-        <v>2</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="3">
-        <v>8</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="3">
-        <v>2</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="3">
-        <v>8</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="3">
-        <v>2</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="3">
-        <v>8</v>
-      </c>
-      <c r="E40" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="3">
-        <v>2</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="3">
-        <v>8</v>
-      </c>
-      <c r="E41" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58">
+        <v>9</v>
+      </c>
+      <c r="E58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B59" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" t="s">
+        <v>73</v>
+      </c>
+      <c r="D59">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="3">
-        <v>2</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="3">
-        <v>8</v>
-      </c>
-      <c r="E42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" s="3">
-        <v>2</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" s="3">
-        <v>8</v>
-      </c>
-      <c r="E43" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" s="3">
-        <v>2</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="3">
-        <v>8</v>
-      </c>
-      <c r="E44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="3">
-        <v>2</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="3">
-        <v>8</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="3">
-        <v>2</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="3">
-        <v>8</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="3">
-        <v>2</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D47" s="3">
-        <v>8</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="3">
-        <v>2</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D48" s="3">
-        <v>9</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="3">
-        <v>2</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="3">
-        <v>9</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="3">
-        <v>2</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" s="3">
-        <v>9</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="7">
-        <v>2</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D51" s="7">
-        <v>9</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="3">
-        <v>2</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D52" s="3">
-        <v>9</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B53" s="3">
-        <v>2</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D53" s="3">
-        <v>9</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B54" s="3">
-        <v>2</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D54" s="3">
-        <v>9</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="3">
-        <v>2</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" s="3">
-        <v>9</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B56" s="3">
-        <v>2</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D56" s="3">
-        <v>9</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B57" s="3">
-        <v>2</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D57" s="3">
-        <v>9</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B58" s="3">
-        <v>2</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" s="3">
-        <v>9</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B59" s="3">
-        <v>2</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="3">
-        <v>9</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B60" s="3">
-        <v>2</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D60" s="3">
-        <v>9</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2879,8 +2838,8 @@
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E54">
-    <sortCondition ref="D1:D54"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E53">
+    <sortCondition ref="D1:D53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2888,6 +2847,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a2b89b45-95bf-4463-8a3d-9dd6e3916c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EA8D7481D231A4FA18CBAA0981A6EC2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc1615ac0acaf52a2064e07cd71218d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a2b89b45-95bf-4463-8a3d-9dd6e3916c62" xmlns:ns4="a72d049a-45c8-472d-b680-4c3738a32d71" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86d3c9ffb2972386f85505747a36cfa" ns3:_="" ns4:_="">
     <xsd:import namespace="a2b89b45-95bf-4463-8a3d-9dd6e3916c62"/>
@@ -3102,38 +3078,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a2b89b45-95bf-4463-8a3d-9dd6e3916c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28DBB848-8EC7-4EC4-AB4B-BFC39248A8FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23917988-726C-494A-9277-B55C7475CFA6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a2b89b45-95bf-4463-8a3d-9dd6e3916c62"/>
-    <ds:schemaRef ds:uri="a72d049a-45c8-472d-b680-4c3738a32d71"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3156,9 +3104,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23917988-726C-494A-9277-B55C7475CFA6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28DBB848-8EC7-4EC4-AB4B-BFC39248A8FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a2b89b45-95bf-4463-8a3d-9dd6e3916c62"/>
+    <ds:schemaRef ds:uri="a72d049a-45c8-472d-b680-4c3738a32d71"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Bugfixes and general improvements
</commit_message>
<xml_diff>
--- a/agquery/Update/Policy_Link.xlsx
+++ b/agquery/Update/Policy_Link.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\R\50x30AQP\agquery\Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altomes\Desktop\50x30_AQP\agquery\Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69C7243-8192-45DF-9CB3-20F09F626FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAC9520-2385-43D0-B2FB-DBC52BB02FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy_Pathways" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="126">
   <si>
     <t>Goal.Id</t>
   </si>
@@ -289,45 +289,15 @@
     <t>Pathway.Id</t>
   </si>
   <si>
-    <t>feed_cattle</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
     <t>irrigation</t>
   </si>
   <si>
-    <t>for_breed_cattle</t>
-  </si>
-  <si>
-    <t>for_draught_cattle</t>
-  </si>
-  <si>
-    <t>vax_pct_cattle</t>
-  </si>
-  <si>
     <t>births_Cattle</t>
   </si>
   <si>
-    <t>mortality_rt_chickens</t>
-  </si>
-  <si>
-    <t>vax_pct_chickens</t>
-  </si>
-  <si>
-    <t>sale_ppkg_chickens</t>
-  </si>
-  <si>
-    <t>mortality_rt_cattle</t>
-  </si>
-  <si>
-    <t>productivity_cattle</t>
-  </si>
-  <si>
-    <t>num_cattle</t>
-  </si>
-  <si>
     <t>drought</t>
   </si>
   <si>
@@ -391,9 +361,6 @@
     <t>trt_vax_spending_Chickens</t>
   </si>
   <si>
-    <t>cur_trt_chickens</t>
-  </si>
-  <si>
     <t>cur_trt_spending_Chickens</t>
   </si>
   <si>
@@ -412,7 +379,52 @@
     <t>cur_trt_spending_Cattle</t>
   </si>
   <si>
-    <t>provision_feed_cattle</t>
+    <t>for_draught_Cattle</t>
+  </si>
+  <si>
+    <t>vax_pct_Cattle</t>
+  </si>
+  <si>
+    <t>mortality_rt_Cattle</t>
+  </si>
+  <si>
+    <t>for_breed_Cattle</t>
+  </si>
+  <si>
+    <t>productivity_Cattle</t>
+  </si>
+  <si>
+    <t>provision_feed_Cattle</t>
+  </si>
+  <si>
+    <t>feed_Cattle</t>
+  </si>
+  <si>
+    <t>Improve farmer access to training on Cattle production (best feeding practices and disease prevention) through government/NGO extension services</t>
+  </si>
+  <si>
+    <t>Improve Cattle productivity and reduce farmer labor on livestock feeding through government-subsidized programs which introduce forage species on smallholder land</t>
+  </si>
+  <si>
+    <t>num_Cattle</t>
+  </si>
+  <si>
+    <t>Improve Cattle production with high intervention programs that provide both subsidies and education to smallholder farmers</t>
+  </si>
+  <si>
+    <t>Indicators associated with Cattle productivity</t>
+  </si>
+  <si>
+    <t>mortality_rt_Chickens</t>
+  </si>
+  <si>
+    <t>vax_pct_Chickens</t>
+  </si>
+  <si>
+    <t>sale_ppkg_Chickens</t>
+  </si>
+  <si>
+    <t>cur_trt_Chickens</t>
   </si>
 </sst>
 </file>
@@ -1798,12 +1810,12 @@
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1816,8 +1828,8 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,7 +1855,7 @@
         <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1860,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1877,7 +1889,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1894,7 +1906,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1911,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1928,7 +1940,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1945,7 +1957,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1962,7 +1974,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1979,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1990,13 +2002,13 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2007,13 +2019,13 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D11">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2024,13 +2036,13 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2041,13 +2053,13 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2058,13 +2070,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2075,13 +2087,13 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D15">
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2098,7 +2110,7 @@
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2115,7 +2127,7 @@
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2132,7 +2144,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2149,7 +2161,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2166,7 +2178,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2183,7 +2195,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2200,7 +2212,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2217,7 +2229,7 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2228,13 +2240,13 @@
         <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D24">
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2245,13 +2257,13 @@
         <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D25">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2262,13 +2274,13 @@
         <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D26">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2279,13 +2291,13 @@
         <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D27">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2296,13 +2308,13 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D28">
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2313,13 +2325,13 @@
         <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D29">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2330,13 +2342,13 @@
         <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D30">
         <v>7</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2347,13 +2359,13 @@
         <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D31">
         <v>7</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2364,13 +2376,13 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D32">
         <v>7</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2381,13 +2393,13 @@
         <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D33">
         <v>7</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2398,13 +2410,13 @@
         <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D34">
         <v>7</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2415,13 +2427,13 @@
         <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D35">
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2432,13 +2444,13 @@
         <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D36">
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2449,13 +2461,13 @@
         <v>48</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D37">
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2466,13 +2478,13 @@
         <v>48</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D38">
         <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2483,13 +2495,13 @@
         <v>48</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D39">
         <v>8</v>
       </c>
       <c r="E39" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2500,13 +2512,13 @@
         <v>48</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D40">
         <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2517,13 +2529,13 @@
         <v>48</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D41">
         <v>8</v>
       </c>
       <c r="E41" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2534,13 +2546,13 @@
         <v>48</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D42">
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2551,13 +2563,13 @@
         <v>48</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D43">
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2568,13 +2580,13 @@
         <v>48</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D44">
         <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2585,13 +2597,13 @@
         <v>48</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D45">
         <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2602,13 +2614,13 @@
         <v>48</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D46">
         <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2619,13 +2631,13 @@
         <v>48</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>50</v>
+        <v>118</v>
       </c>
       <c r="D47">
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2636,13 +2648,13 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="D48">
         <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2653,13 +2665,13 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="D49">
         <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2670,13 +2682,13 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D50">
         <v>9</v>
       </c>
       <c r="E50" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2687,13 +2699,13 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D51">
         <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2704,13 +2716,13 @@
         <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D52">
         <v>9</v>
       </c>
       <c r="E52" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2721,13 +2733,13 @@
         <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D53">
         <v>9</v>
       </c>
       <c r="E53" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2738,13 +2750,13 @@
         <v>48</v>
       </c>
       <c r="C54" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D54">
         <v>9</v>
       </c>
       <c r="E54" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2755,13 +2767,13 @@
         <v>48</v>
       </c>
       <c r="C55" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D55">
         <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2772,13 +2784,13 @@
         <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D56">
         <v>9</v>
       </c>
       <c r="E56" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2789,13 +2801,13 @@
         <v>48</v>
       </c>
       <c r="C57" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D57">
         <v>9</v>
       </c>
       <c r="E57" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2806,13 +2818,13 @@
         <v>48</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D58">
         <v>9</v>
       </c>
       <c r="E58" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2823,13 +2835,13 @@
         <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D59">
         <v>9</v>
       </c>
       <c r="E59" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2847,23 +2859,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a2b89b45-95bf-4463-8a3d-9dd6e3916c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EA8D7481D231A4FA18CBAA0981A6EC2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dc1615ac0acaf52a2064e07cd71218d4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a2b89b45-95bf-4463-8a3d-9dd6e3916c62" xmlns:ns4="a72d049a-45c8-472d-b680-4c3738a32d71" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86d3c9ffb2972386f85505747a36cfa" ns3:_="" ns4:_="">
     <xsd:import namespace="a2b89b45-95bf-4463-8a3d-9dd6e3916c62"/>
@@ -3078,10 +3073,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a2b89b45-95bf-4463-8a3d-9dd6e3916c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23917988-726C-494A-9277-B55C7475CFA6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28DBB848-8EC7-4EC4-AB4B-BFC39248A8FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a2b89b45-95bf-4463-8a3d-9dd6e3916c62"/>
+    <ds:schemaRef ds:uri="a72d049a-45c8-472d-b680-4c3738a32d71"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3104,20 +3127,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28DBB848-8EC7-4EC4-AB4B-BFC39248A8FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23917988-726C-494A-9277-B55C7475CFA6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a2b89b45-95bf-4463-8a3d-9dd6e3916c62"/>
-    <ds:schemaRef ds:uri="a72d049a-45c8-472d-b680-4c3738a32d71"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>